<commit_message>
bug fix + add data and menu for full date range
</commit_message>
<xml_diff>
--- a/data/excel_files/FormattedDec2022.xlsx
+++ b/data/excel_files/FormattedDec2022.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -50,8 +50,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -93,7 +94,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -117,6 +118,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -2656,43 +2660,123 @@
       </c>
     </row>
     <row r="114">
+      <c r="A114" s="9">
+        <v>44924.0</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E114" s="5">
         <v>40.0</v>
       </c>
     </row>
     <row r="115">
+      <c r="A115" s="9">
+        <v>44924.0</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E115" s="5">
         <v>60.0</v>
       </c>
     </row>
     <row r="116">
+      <c r="A116" s="9">
+        <v>44924.0</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E116" s="5">
         <v>25.0</v>
       </c>
     </row>
     <row r="117">
+      <c r="A117" s="9">
+        <v>44924.0</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E117" s="5">
         <v>60.0</v>
       </c>
     </row>
     <row r="118">
+      <c r="A118" s="9">
+        <v>44925.0</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E118" s="5">
         <v>40.0</v>
       </c>
     </row>
     <row r="119">
+      <c r="A119" s="9">
+        <v>44925.0</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E119" s="5">
         <v>60.0</v>
       </c>
     </row>
     <row r="120">
+      <c r="A120" s="9">
+        <v>44925.0</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E120" s="5">
         <v>25.0</v>
       </c>
     </row>
     <row r="121">
+      <c r="A121" s="9">
+        <v>44925.0</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E121" s="5">
         <v>70.0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="9">
+        <v>44926.0</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="9">
+        <v>44926.0</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="9">
+        <v>44926.0</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="9">
+        <v>44926.0</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>